<commit_message>
Tried to rethink part of the random-chance model formulation based on data from Nunney & Muir (2015); doesn't seem very successful so far. Python file, random-chance-model.py has other details about this formulation, and the data used.
</commit_message>
<xml_diff>
--- a/all-data/v1-data/22Oct2018/linear-v1-multipop-crude-rate-n.xlsx
+++ b/all-data/v1-data/22Oct2018/linear-v1-multipop-crude-rate-n.xlsx
@@ -15,9 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
     <t>Cell number</t>
+  </si>
+  <si>
+    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -885,103 +888,103 @@
         <v>0</v>
       </c>
       <c r="BQ2" t="n">
-        <v>1</v>
+        <v>1.000100010001</v>
       </c>
       <c r="BR2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY2" t="n">
-        <v>2</v>
+        <v>1.000200040008002</v>
       </c>
       <c r="BZ2" t="n">
-        <v>3</v>
+        <v>1.000300090027008</v>
       </c>
       <c r="CA2" t="n">
-        <v>4</v>
+        <v>1.000400160064026</v>
       </c>
       <c r="CB2" t="n">
-        <v>5</v>
+        <v>1.000500250125063</v>
       </c>
       <c r="CC2" t="n">
-        <v>7</v>
+        <v>2.001400980686481</v>
       </c>
       <c r="CD2" t="n">
-        <v>8</v>
+        <v>1.00080064051241</v>
       </c>
       <c r="CE2" t="n">
-        <v>9</v>
+        <v>1.000900810729657</v>
       </c>
       <c r="CF2" t="n">
-        <v>12</v>
+        <v>3.003604325190228</v>
       </c>
       <c r="CG2" t="n">
-        <v>13</v>
+        <v>1.00130169219986</v>
       </c>
       <c r="CH2" t="n">
-        <v>16</v>
+        <v>3.004807692307693</v>
       </c>
       <c r="CI2" t="n">
-        <v>18</v>
+        <v>2.003606491685033</v>
       </c>
       <c r="CJ2" t="n">
-        <v>19</v>
+        <v>1.001903616872057</v>
       </c>
       <c r="CK2" t="n">
-        <v>23</v>
+        <v>4.009221208780195</v>
       </c>
       <c r="CL2" t="n">
-        <v>27</v>
+        <v>4.010829238945152</v>
       </c>
       <c r="CM2" t="n">
-        <v>31</v>
+        <v>4.012438559534557</v>
       </c>
       <c r="CN2" t="n">
-        <v>38</v>
+        <v>7.026701465569163</v>
       </c>
       <c r="CO2" t="n">
-        <v>43</v>
+        <v>5.021592849251783</v>
       </c>
       <c r="CP2" t="n">
-        <v>54</v>
+        <v>11.05972250150814</v>
       </c>
       <c r="CQ2" t="n">
-        <v>60</v>
+        <v>6.036217303822937</v>
       </c>
       <c r="CR2" t="n">
-        <v>67</v>
+        <v>7.047216349541931</v>
       </c>
       <c r="CS2" t="n">
-        <v>74</v>
+        <v>7.052186177715091</v>
       </c>
       <c r="CT2" t="n">
-        <v>89</v>
+        <v>15.13469881949349</v>
       </c>
       <c r="CU2" t="n">
-        <v>94</v>
+        <v>5.047445992327882</v>
       </c>
       <c r="CV2" t="n">
-        <v>104</v>
+        <v>10.1050929668553</v>
       </c>
       <c r="CW2" t="n">
-        <v>118</v>
+        <v>14.16717263711799</v>
       </c>
     </row>
     <row r="3" spans="1:101">
@@ -1142,151 +1145,151 @@
         <v>0</v>
       </c>
       <c r="BA3" t="n">
-        <v>1</v>
+        <v>1.000100010001</v>
       </c>
       <c r="BB3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE3" t="n">
-        <v>3</v>
+        <v>2.000600180054016</v>
       </c>
       <c r="BF3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BG3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BI3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BJ3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BK3" t="n">
-        <v>4</v>
+        <v>1.000400160064026</v>
       </c>
       <c r="BL3" t="n">
-        <v>5</v>
+        <v>1.000500250125063</v>
       </c>
       <c r="BM3" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BN3" t="n">
-        <v>6</v>
+        <v>1.00060036021613</v>
       </c>
       <c r="BO3" t="n">
-        <v>7</v>
+        <v>1.00070049034324</v>
       </c>
       <c r="BP3" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="BQ3" t="n">
-        <v>10</v>
+        <v>3.003003003003003</v>
       </c>
       <c r="BR3" t="n">
-        <v>15</v>
+        <v>5.00751126690035</v>
       </c>
       <c r="BS3" t="n">
-        <v>16</v>
+        <v>1.001602564102564</v>
       </c>
       <c r="BT3" t="n">
-        <v>18</v>
+        <v>2.003606491685033</v>
       </c>
       <c r="BU3" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="BV3" t="n">
-        <v>20</v>
+        <v>2.004008016032064</v>
       </c>
       <c r="BW3" t="n">
-        <v>22</v>
+        <v>2.004409701342955</v>
       </c>
       <c r="BX3" t="n">
-        <v>25</v>
+        <v>3.007518796992481</v>
       </c>
       <c r="BY3" t="n">
-        <v>27</v>
+        <v>2.005414619472576</v>
       </c>
       <c r="BZ3" t="n">
-        <v>32</v>
+        <v>5.01605136436597</v>
       </c>
       <c r="CA3" t="n">
-        <v>36</v>
+        <v>4.014452027298274</v>
       </c>
       <c r="CB3" t="n">
-        <v>40</v>
+        <v>4.016064257028113</v>
       </c>
       <c r="CC3" t="n">
-        <v>43</v>
+        <v>3.01295570955107</v>
       </c>
       <c r="CD3" t="n">
-        <v>47</v>
+        <v>4.01888877725309</v>
       </c>
       <c r="CE3" t="n">
-        <v>56</v>
+        <v>9.050683829444891</v>
       </c>
       <c r="CF3" t="n">
-        <v>60</v>
+        <v>4.024144869215291</v>
       </c>
       <c r="CG3" t="n">
-        <v>72</v>
+        <v>12.0870265914585</v>
       </c>
       <c r="CH3" t="n">
-        <v>88</v>
+        <v>16.14205004035512</v>
       </c>
       <c r="CI3" t="n">
-        <v>108</v>
+        <v>20.21835826930853</v>
       </c>
       <c r="CJ3" t="n">
-        <v>126</v>
+        <v>18.22969414624266</v>
       </c>
       <c r="CK3" t="n">
-        <v>140</v>
+        <v>14.19878296146045</v>
       </c>
       <c r="CL3" t="n">
-        <v>161</v>
+        <v>21.34363248297591</v>
       </c>
       <c r="CM3" t="n">
-        <v>176</v>
+        <v>15.26872964169381</v>
       </c>
       <c r="CN3" t="n">
-        <v>196</v>
+        <v>20.39983680130559</v>
       </c>
       <c r="CO3" t="n">
-        <v>228</v>
+        <v>32.74662300450266</v>
       </c>
       <c r="CP3" t="n">
-        <v>243</v>
+        <v>15.37357794404018</v>
       </c>
       <c r="CQ3" t="n">
-        <v>285</v>
+        <v>43.23211528564077</v>
       </c>
       <c r="CR3" t="n">
-        <v>317</v>
+        <v>33.04760921202107</v>
       </c>
       <c r="CS3" t="n">
-        <v>351</v>
+        <v>35.23681210488133</v>
       </c>
       <c r="CT3" t="n">
-        <v>393</v>
+        <v>43.71812220256064</v>
       </c>
       <c r="CU3" t="n">
-        <v>429</v>
+        <v>37.61362449064884</v>
       </c>
       <c r="CV3" t="n">
-        <v>479</v>
+        <v>52.5154920701607</v>
       </c>
       <c r="CW3" t="n">
-        <v>529</v>
+        <v>52.79273571956499</v>
       </c>
     </row>
     <row r="4" spans="1:101">
@@ -1450,148 +1453,148 @@
         <v>0</v>
       </c>
       <c r="BB4" t="n">
-        <v>1</v>
+        <v>1.000100010001</v>
       </c>
       <c r="BC4" t="n">
-        <v>2</v>
+        <v>1.000200040008002</v>
       </c>
       <c r="BD4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BE4" t="n">
-        <v>3</v>
+        <v>1.000300090027008</v>
       </c>
       <c r="BF4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BG4" t="n">
-        <v>4</v>
+        <v>1.000400160064026</v>
       </c>
       <c r="BH4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BI4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BJ4" t="n">
-        <v>5</v>
+        <v>1.000500250125063</v>
       </c>
       <c r="BK4" t="n">
-        <v>9</v>
+        <v>4.003603242918627</v>
       </c>
       <c r="BL4" t="n">
-        <v>12</v>
+        <v>3.003604325190228</v>
       </c>
       <c r="BM4" t="n">
-        <v>14</v>
+        <v>2.002803925495694</v>
       </c>
       <c r="BN4" t="n">
-        <v>19</v>
+        <v>5.009518084360284</v>
       </c>
       <c r="BO4" t="n">
-        <v>26</v>
+        <v>7.018247443352717</v>
       </c>
       <c r="BP4" t="n">
-        <v>32</v>
+        <v>6.019261637239165</v>
       </c>
       <c r="BQ4" t="n">
-        <v>37</v>
+        <v>5.01856870420556</v>
       </c>
       <c r="BR4" t="n">
-        <v>43</v>
+        <v>6.025911419102139</v>
       </c>
       <c r="BS4" t="n">
-        <v>47</v>
+        <v>4.01888877725309</v>
       </c>
       <c r="BT4" t="n">
-        <v>54</v>
+        <v>7.038005228232455</v>
       </c>
       <c r="BU4" t="n">
-        <v>59</v>
+        <v>5.029675082989639</v>
       </c>
       <c r="BV4" t="n">
-        <v>72</v>
+        <v>13.09427880741338</v>
       </c>
       <c r="BW4" t="n">
-        <v>84</v>
+        <v>12.10165389269867</v>
       </c>
       <c r="BX4" t="n">
-        <v>98</v>
+        <v>14.13855786709756</v>
       </c>
       <c r="BY4" t="n">
-        <v>119</v>
+        <v>21.25290962453193</v>
       </c>
       <c r="BZ4" t="n">
-        <v>134</v>
+        <v>15.20372998175553</v>
       </c>
       <c r="CA4" t="n">
-        <v>161</v>
+        <v>27.4418131923976</v>
       </c>
       <c r="CB4" t="n">
-        <v>183</v>
+        <v>22.41010492003667</v>
       </c>
       <c r="CC4" t="n">
-        <v>216</v>
+        <v>33.72853638593622</v>
       </c>
       <c r="CD4" t="n">
-        <v>254</v>
+        <v>38.99035501744305</v>
       </c>
       <c r="CE4" t="n">
-        <v>290</v>
+        <v>37.07518022657055</v>
       </c>
       <c r="CF4" t="n">
-        <v>343</v>
+        <v>54.88246867557212</v>
       </c>
       <c r="CG4" t="n">
-        <v>381</v>
+        <v>39.50514606507953</v>
       </c>
       <c r="CH4" t="n">
-        <v>443</v>
+        <v>64.87391440828712</v>
       </c>
       <c r="CI4" t="n">
-        <v>485</v>
+        <v>44.1408302679979</v>
       </c>
       <c r="CJ4" t="n">
-        <v>533</v>
+        <v>50.70244005492764</v>
       </c>
       <c r="CK4" t="n">
-        <v>589</v>
+        <v>59.50483476782489</v>
       </c>
       <c r="CL4" t="n">
-        <v>677</v>
+        <v>94.39021774107046</v>
       </c>
       <c r="CM4" t="n">
-        <v>753</v>
+        <v>82.18881799502542</v>
       </c>
       <c r="CN4" t="n">
-        <v>838</v>
+        <v>92.77450338354072</v>
       </c>
       <c r="CO4" t="n">
-        <v>934</v>
+        <v>105.8901389808074</v>
       </c>
       <c r="CP4" t="n">
-        <v>1019</v>
+        <v>94.64424897004787</v>
       </c>
       <c r="CQ4" t="n">
-        <v>1120</v>
+        <v>113.7387387387387</v>
       </c>
       <c r="CR4" t="n">
-        <v>1246</v>
+        <v>143.9342015078821</v>
       </c>
       <c r="CS4" t="n">
-        <v>1348</v>
+        <v>117.8918169209431</v>
       </c>
       <c r="CT4" t="n">
-        <v>1473</v>
+        <v>146.5931746217896</v>
       </c>
       <c r="CU4" t="n">
-        <v>1614</v>
+        <v>168.1373718101598</v>
       </c>
       <c r="CV4" t="n">
-        <v>1758</v>
+        <v>174.7148750303325</v>
       </c>
       <c r="CW4" t="n">
-        <v>1907</v>
+        <v>184.1097244532312</v>
       </c>
     </row>
     <row r="5" spans="1:101">
@@ -1701,202 +1704,202 @@
         <v>0</v>
       </c>
       <c r="AJ5" t="n">
-        <v>1</v>
+        <v>1.000100010001</v>
       </c>
       <c r="AK5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX5" t="n">
-        <v>2</v>
+        <v>1.000200040008002</v>
       </c>
       <c r="AY5" t="n">
-        <v>3</v>
+        <v>1.000300090027008</v>
       </c>
       <c r="AZ5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BA5" t="n">
-        <v>4</v>
+        <v>1.000400160064026</v>
       </c>
       <c r="BB5" t="n">
-        <v>9</v>
+        <v>5.004504053648283</v>
       </c>
       <c r="BC5" t="n">
-        <v>10</v>
+        <v>1.001001001001001</v>
       </c>
       <c r="BD5" t="n">
-        <v>12</v>
+        <v>2.002402883460152</v>
       </c>
       <c r="BE5" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="BF5" t="n">
-        <v>14</v>
+        <v>2.002803925495694</v>
       </c>
       <c r="BG5" t="n">
-        <v>19</v>
+        <v>5.009518084360284</v>
       </c>
       <c r="BH5" t="n">
-        <v>28</v>
+        <v>9.025270758122744</v>
       </c>
       <c r="BI5" t="n">
-        <v>33</v>
+        <v>5.016554630279924</v>
       </c>
       <c r="BJ5" t="n">
-        <v>40</v>
+        <v>7.028112449799197</v>
       </c>
       <c r="BK5" t="n">
-        <v>46</v>
+        <v>6.027727546714888</v>
       </c>
       <c r="BL5" t="n">
-        <v>60</v>
+        <v>14.08450704225352</v>
       </c>
       <c r="BM5" t="n">
-        <v>72</v>
+        <v>12.0870265914585</v>
       </c>
       <c r="BN5" t="n">
-        <v>96</v>
+        <v>24.23263327948304</v>
       </c>
       <c r="BO5" t="n">
-        <v>113</v>
+        <v>17.19429553959745</v>
       </c>
       <c r="BP5" t="n">
-        <v>127</v>
+        <v>14.18008710624937</v>
       </c>
       <c r="BQ5" t="n">
-        <v>154</v>
+        <v>27.42230347349177</v>
       </c>
       <c r="BR5" t="n">
-        <v>189</v>
+        <v>35.67424319641219</v>
       </c>
       <c r="BS5" t="n">
-        <v>222</v>
+        <v>33.74923297197791</v>
       </c>
       <c r="BT5" t="n">
-        <v>263</v>
+        <v>42.10742528499537</v>
       </c>
       <c r="BU5" t="n">
-        <v>309</v>
+        <v>47.46672170054691</v>
       </c>
       <c r="BV5" t="n">
-        <v>364</v>
+        <v>57.07762557077626</v>
       </c>
       <c r="BW5" t="n">
-        <v>412</v>
+        <v>50.06257822277848</v>
       </c>
       <c r="BX5" t="n">
-        <v>470</v>
+        <v>60.8604407135362</v>
       </c>
       <c r="BY5" t="n">
-        <v>543</v>
+        <v>77.19149836100243</v>
       </c>
       <c r="BZ5" t="n">
-        <v>624</v>
+        <v>86.39078498293516</v>
       </c>
       <c r="CA5" t="n">
-        <v>700</v>
+        <v>81.72043010752689</v>
       </c>
       <c r="CB5" t="n">
-        <v>776</v>
+        <v>82.3937554206418</v>
       </c>
       <c r="CC5" t="n">
-        <v>883</v>
+        <v>117.3631677086761</v>
       </c>
       <c r="CD5" t="n">
-        <v>1003</v>
+        <v>133.3777925975325</v>
       </c>
       <c r="CE5" t="n">
-        <v>1144</v>
+        <v>159.2140921409214</v>
       </c>
       <c r="CF5" t="n">
-        <v>1255</v>
+        <v>126.9296740994854</v>
       </c>
       <c r="CG5" t="n">
-        <v>1398</v>
+        <v>166.2404092071612</v>
       </c>
       <c r="CH5" t="n">
-        <v>1566</v>
+        <v>199.1937396253261</v>
       </c>
       <c r="CI5" t="n">
-        <v>1753</v>
+        <v>226.7491208924457</v>
       </c>
       <c r="CJ5" t="n">
-        <v>1939</v>
+        <v>230.7406029028656</v>
       </c>
       <c r="CK5" t="n">
-        <v>2144</v>
+        <v>260.9470468431772</v>
       </c>
       <c r="CL5" t="n">
-        <v>2346</v>
+        <v>263.9142931800366</v>
       </c>
       <c r="CM5" t="n">
-        <v>2556</v>
+        <v>282.1063944116067</v>
       </c>
       <c r="CN5" t="n">
-        <v>2786</v>
+        <v>318.824507901303</v>
       </c>
       <c r="CO5" t="n">
-        <v>3045</v>
+        <v>372.3939611790079</v>
       </c>
       <c r="CP5" t="n">
-        <v>3274</v>
+        <v>340.4698186143324</v>
       </c>
       <c r="CQ5" t="n">
-        <v>3511</v>
+        <v>365.2334720295885</v>
       </c>
       <c r="CR5" t="n">
-        <v>3762</v>
+        <v>402.3725553061879</v>
       </c>
       <c r="CS5" t="n">
-        <v>4039</v>
+        <v>464.6871330313706</v>
       </c>
       <c r="CT5" t="n">
-        <v>4300</v>
+        <v>457.8947368421053</v>
       </c>
       <c r="CU5" t="n">
-        <v>4582</v>
+        <v>520.4872646733112</v>
       </c>
       <c r="CV5" t="n">
-        <v>4840</v>
+        <v>500</v>
       </c>
       <c r="CW5" t="n">
-        <v>5118</v>
+        <v>569.4387546087669</v>
       </c>
     </row>
     <row r="6" spans="1:101">
@@ -2003,205 +2006,205 @@
         <v>0</v>
       </c>
       <c r="AI6" t="n">
-        <v>1</v>
+        <v>1.000100010001</v>
       </c>
       <c r="AJ6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR6" t="n">
-        <v>2</v>
+        <v>1.000200040008002</v>
       </c>
       <c r="AS6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT6" t="n">
-        <v>4</v>
+        <v>2.000800320128052</v>
       </c>
       <c r="AU6" t="n">
-        <v>5</v>
+        <v>1.000500250125063</v>
       </c>
       <c r="AV6" t="n">
-        <v>8</v>
+        <v>3.00240192153723</v>
       </c>
       <c r="AW6" t="n">
-        <v>11</v>
+        <v>3.003303633997398</v>
       </c>
       <c r="AX6" t="n">
-        <v>15</v>
+        <v>4.006009013520281</v>
       </c>
       <c r="AY6" t="n">
-        <v>19</v>
+        <v>4.007614467488227</v>
       </c>
       <c r="AZ6" t="n">
-        <v>25</v>
+        <v>6.015037593984962</v>
       </c>
       <c r="BA6" t="n">
-        <v>28</v>
+        <v>3.008423586040915</v>
       </c>
       <c r="BB6" t="n">
-        <v>37</v>
+        <v>9.033423667570009</v>
       </c>
       <c r="BC6" t="n">
-        <v>42</v>
+        <v>5.021088572002411</v>
       </c>
       <c r="BD6" t="n">
-        <v>53</v>
+        <v>11.05861063637278</v>
       </c>
       <c r="BE6" t="n">
-        <v>69</v>
+        <v>16.11116705266338</v>
       </c>
       <c r="BF6" t="n">
-        <v>83</v>
+        <v>14.11717253201573</v>
       </c>
       <c r="BG6" t="n">
-        <v>113</v>
+        <v>30.34287448164256</v>
       </c>
       <c r="BH6" t="n">
-        <v>131</v>
+        <v>18.23892998277434</v>
       </c>
       <c r="BI6" t="n">
-        <v>156</v>
+        <v>25.39618041446566</v>
       </c>
       <c r="BJ6" t="n">
-        <v>197</v>
+        <v>41.82393144955626</v>
       </c>
       <c r="BK6" t="n">
-        <v>235</v>
+        <v>38.91449052739375</v>
       </c>
       <c r="BL6" t="n">
-        <v>271</v>
+        <v>37.00277520814061</v>
       </c>
       <c r="BM6" t="n">
-        <v>337</v>
+        <v>68.30176963675878</v>
       </c>
       <c r="BN6" t="n">
-        <v>396</v>
+        <v>61.43273635985006</v>
       </c>
       <c r="BO6" t="n">
-        <v>463</v>
+        <v>70.25270001048548</v>
       </c>
       <c r="BP6" t="n">
-        <v>541</v>
+        <v>82.46114811290833</v>
       </c>
       <c r="BQ6" t="n">
-        <v>629</v>
+        <v>93.90673353964358</v>
       </c>
       <c r="BR6" t="n">
-        <v>721</v>
+        <v>99.14861515249488</v>
       </c>
       <c r="BS6" t="n">
-        <v>821</v>
+        <v>108.9443294476523</v>
       </c>
       <c r="BT6" t="n">
-        <v>930</v>
+        <v>120.1764057331863</v>
       </c>
       <c r="BU6" t="n">
-        <v>1062</v>
+        <v>147.6840456477959</v>
       </c>
       <c r="BV6" t="n">
-        <v>1206</v>
+        <v>163.7480100068228</v>
       </c>
       <c r="BW6" t="n">
-        <v>1362</v>
+        <v>180.5973605001158</v>
       </c>
       <c r="BX6" t="n">
-        <v>1505</v>
+        <v>168.3343143025309</v>
       </c>
       <c r="BY6" t="n">
-        <v>1689</v>
+        <v>221.3933341354831</v>
       </c>
       <c r="BZ6" t="n">
-        <v>1896</v>
+        <v>255.4294175715696</v>
       </c>
       <c r="CA6" t="n">
-        <v>2087</v>
+        <v>241.3749526096297</v>
       </c>
       <c r="CB6" t="n">
-        <v>2318</v>
+        <v>300.7029419422025</v>
       </c>
       <c r="CC6" t="n">
-        <v>2574</v>
+        <v>344.7347158631834</v>
       </c>
       <c r="CD6" t="n">
-        <v>2863</v>
+        <v>404.9320442763066</v>
       </c>
       <c r="CE6" t="n">
-        <v>3154</v>
+        <v>425.0657318141981</v>
       </c>
       <c r="CF6" t="n">
-        <v>3441</v>
+        <v>437.5667022411953</v>
       </c>
       <c r="CG6" t="n">
-        <v>3775</v>
+        <v>536.5461847389558</v>
       </c>
       <c r="CH6" t="n">
-        <v>4077</v>
+        <v>509.8767516461253</v>
       </c>
       <c r="CI6" t="n">
-        <v>4407</v>
+        <v>590.0232433398892</v>
       </c>
       <c r="CJ6" t="n">
-        <v>4720</v>
+        <v>592.8030303030303</v>
       </c>
       <c r="CK6" t="n">
-        <v>5061</v>
+        <v>690.4231625835189</v>
       </c>
       <c r="CL6" t="n">
-        <v>5372</v>
+        <v>671.9965427830596</v>
       </c>
       <c r="CM6" t="n">
-        <v>5745</v>
+        <v>876.6157461809636</v>
       </c>
       <c r="CN6" t="n">
-        <v>6106</v>
+        <v>927.0672829994863</v>
       </c>
       <c r="CO6" t="n">
-        <v>6432</v>
+        <v>913.677130044843</v>
       </c>
       <c r="CP6" t="n">
-        <v>6774</v>
+        <v>1060.136391816491</v>
       </c>
       <c r="CQ6" t="n">
-        <v>7041</v>
+        <v>902.3318688746199</v>
       </c>
       <c r="CR6" t="n">
-        <v>7330</v>
+        <v>1082.397003745318</v>
       </c>
       <c r="CS6" t="n">
-        <v>7600</v>
+        <v>1125</v>
       </c>
       <c r="CT6" t="n">
-        <v>7860</v>
+        <v>1214.953271028037</v>
       </c>
       <c r="CU6" t="n">
-        <v>8113</v>
+        <v>1340.752517223106</v>
       </c>
       <c r="CV6" t="n">
-        <v>8360</v>
+        <v>1506.09756097561</v>
       </c>
       <c r="CW6" t="n">
-        <v>8567</v>
+        <v>1444.521981856246</v>
       </c>
     </row>
     <row r="7" spans="1:101">
@@ -2323,190 +2326,190 @@
         <v>0</v>
       </c>
       <c r="AN7" t="n">
-        <v>2</v>
+        <v>2.000400080016003</v>
       </c>
       <c r="AO7" t="n">
-        <v>3</v>
+        <v>1.000300090027008</v>
       </c>
       <c r="AP7" t="n">
-        <v>4</v>
+        <v>1.000400160064026</v>
       </c>
       <c r="AQ7" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AR7" t="n">
-        <v>6</v>
+        <v>2.001200720432259</v>
       </c>
       <c r="AS7" t="n">
-        <v>11</v>
+        <v>5.005506056662329</v>
       </c>
       <c r="AT7" t="n">
-        <v>17</v>
+        <v>6.010217369528198</v>
       </c>
       <c r="AU7" t="n">
-        <v>23</v>
+        <v>6.013831813170292</v>
       </c>
       <c r="AV7" t="n">
-        <v>32</v>
+        <v>9.028892455858749</v>
       </c>
       <c r="AW7" t="n">
-        <v>39</v>
+        <v>7.027406886858749</v>
       </c>
       <c r="AX7" t="n">
-        <v>48</v>
+        <v>9.043408360128616</v>
       </c>
       <c r="AY7" t="n">
-        <v>58</v>
+        <v>10.05833836250251</v>
       </c>
       <c r="AZ7" t="n">
-        <v>79</v>
+        <v>21.1672210462655</v>
       </c>
       <c r="BA7" t="n">
-        <v>102</v>
+        <v>23.23701757930895</v>
       </c>
       <c r="BB7" t="n">
-        <v>129</v>
+        <v>27.35285178806605</v>
       </c>
       <c r="BC7" t="n">
-        <v>168</v>
+        <v>39.66639544344996</v>
       </c>
       <c r="BD7" t="n">
-        <v>219</v>
+        <v>52.14190778039055</v>
       </c>
       <c r="BE7" t="n">
-        <v>260</v>
+        <v>42.09445585215606</v>
       </c>
       <c r="BF7" t="n">
-        <v>316</v>
+        <v>57.82734407269724</v>
       </c>
       <c r="BG7" t="n">
-        <v>380</v>
+        <v>66.52806652806653</v>
       </c>
       <c r="BH7" t="n">
-        <v>454</v>
+        <v>77.51937984496124</v>
       </c>
       <c r="BI7" t="n">
-        <v>545</v>
+        <v>96.2453728186145</v>
       </c>
       <c r="BJ7" t="n">
-        <v>645</v>
+        <v>106.8947087119188</v>
       </c>
       <c r="BK7" t="n">
-        <v>752</v>
+        <v>115.7006920415225</v>
       </c>
       <c r="BL7" t="n">
-        <v>873</v>
+        <v>132.5736824805522</v>
       </c>
       <c r="BM7" t="n">
-        <v>1005</v>
+        <v>146.7481934408004</v>
       </c>
       <c r="BN7" t="n">
-        <v>1161</v>
+        <v>176.4905532300034</v>
       </c>
       <c r="BO7" t="n">
-        <v>1342</v>
+        <v>209.055209055209</v>
       </c>
       <c r="BP7" t="n">
-        <v>1551</v>
+        <v>247.3665522547047</v>
       </c>
       <c r="BQ7" t="n">
-        <v>1749</v>
+        <v>239.9709126166525</v>
       </c>
       <c r="BR7" t="n">
-        <v>1963</v>
+        <v>266.2685081498071</v>
       </c>
       <c r="BS7" t="n">
-        <v>2196</v>
+        <v>298.5648385443362</v>
       </c>
       <c r="BT7" t="n">
-        <v>2440</v>
+        <v>322.7513227513228</v>
       </c>
       <c r="BU7" t="n">
-        <v>2733</v>
+        <v>403.1925141048576</v>
       </c>
       <c r="BV7" t="n">
-        <v>3069</v>
+        <v>484.7785312364738</v>
       </c>
       <c r="BW7" t="n">
-        <v>3379</v>
+        <v>468.2072194532548</v>
       </c>
       <c r="BX7" t="n">
-        <v>3751</v>
+        <v>595.2952472395583</v>
       </c>
       <c r="BY7" t="n">
-        <v>4105</v>
+        <v>600.5089058524173</v>
       </c>
       <c r="BZ7" t="n">
-        <v>4441</v>
+        <v>604.4252563410686</v>
       </c>
       <c r="CA7" t="n">
-        <v>4791</v>
+        <v>671.9139950086389</v>
       </c>
       <c r="CB7" t="n">
-        <v>5165</v>
+        <v>773.5263702171665</v>
       </c>
       <c r="CC7" t="n">
-        <v>5500</v>
+        <v>744.4444444444443</v>
       </c>
       <c r="CD7" t="n">
-        <v>5888</v>
+        <v>943.5797665369649</v>
       </c>
       <c r="CE7" t="n">
-        <v>6279</v>
+        <v>1050.792797635044</v>
       </c>
       <c r="CF7" t="n">
-        <v>6638</v>
+        <v>1067.816775728733</v>
       </c>
       <c r="CG7" t="n">
-        <v>6943</v>
+        <v>997.7101733725875</v>
       </c>
       <c r="CH7" t="n">
-        <v>7290</v>
+        <v>1280.442804428044</v>
       </c>
       <c r="CI7" t="n">
-        <v>7589</v>
+        <v>1240.149315636665</v>
       </c>
       <c r="CJ7" t="n">
-        <v>7885</v>
+        <v>1399.527186761229</v>
       </c>
       <c r="CK7" t="n">
-        <v>8157</v>
+        <v>1475.854584915898</v>
       </c>
       <c r="CL7" t="n">
-        <v>8436</v>
+        <v>1783.88746803069</v>
       </c>
       <c r="CM7" t="n">
-        <v>8653</v>
+        <v>1610.987379361544</v>
       </c>
       <c r="CN7" t="n">
-        <v>8862</v>
+        <v>1836.555360281195</v>
       </c>
       <c r="CO7" t="n">
-        <v>9073</v>
+        <v>2276.159654800431</v>
       </c>
       <c r="CP7" t="n">
-        <v>9234</v>
+        <v>2101.827676240209</v>
       </c>
       <c r="CQ7" t="n">
-        <v>9376</v>
+        <v>2275.641025641025</v>
       </c>
       <c r="CR7" t="n">
-        <v>9492</v>
+        <v>2283.464566929134</v>
       </c>
       <c r="CS7" t="n">
-        <v>9598</v>
+        <v>2636.81592039801</v>
       </c>
       <c r="CT7" t="n">
-        <v>9696</v>
+        <v>3223.684210526316</v>
       </c>
       <c r="CU7" t="n">
-        <v>9769</v>
+        <v>3160.17316017316</v>
       </c>
       <c r="CV7" t="n">
-        <v>9822</v>
+        <v>2977.52808988764</v>
       </c>
       <c r="CW7" t="n">
-        <v>9855</v>
+        <v>2275.862068965517</v>
       </c>
     </row>
     <row r="8" spans="1:101">
@@ -2592,226 +2595,226 @@
         <v>0</v>
       </c>
       <c r="AB8" t="n">
-        <v>1</v>
+        <v>1.000100010001</v>
       </c>
       <c r="AC8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG8" t="n">
-        <v>2</v>
+        <v>1.000200040008002</v>
       </c>
       <c r="AH8" t="n">
-        <v>3</v>
+        <v>1.000300090027008</v>
       </c>
       <c r="AI8" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ8" t="n">
-        <v>4</v>
+        <v>1.000400160064026</v>
       </c>
       <c r="AK8" t="n">
-        <v>5</v>
+        <v>1.000500250125063</v>
       </c>
       <c r="AL8" t="n">
-        <v>8</v>
+        <v>3.00240192153723</v>
       </c>
       <c r="AM8" t="n">
-        <v>10</v>
+        <v>2.002002002002002</v>
       </c>
       <c r="AN8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AO8" t="n">
-        <v>13</v>
+        <v>3.00390507659958</v>
       </c>
       <c r="AP8" t="n">
-        <v>24</v>
+        <v>11.02646351242983</v>
       </c>
       <c r="AQ8" t="n">
-        <v>37</v>
+        <v>13.04827863093446</v>
       </c>
       <c r="AR8" t="n">
-        <v>48</v>
+        <v>11.05305466237942</v>
       </c>
       <c r="AS8" t="n">
-        <v>61</v>
+        <v>13.07978669886306</v>
       </c>
       <c r="AT8" t="n">
-        <v>79</v>
+        <v>18.14333232537043</v>
       </c>
       <c r="AU8" t="n">
-        <v>101</v>
+        <v>22.22446711789069</v>
       </c>
       <c r="AV8" t="n">
-        <v>122</v>
+        <v>21.25936424377404</v>
       </c>
       <c r="AW8" t="n">
-        <v>154</v>
+        <v>32.50050782043469</v>
       </c>
       <c r="AX8" t="n">
-        <v>192</v>
+        <v>38.74388254486134</v>
       </c>
       <c r="AY8" t="n">
-        <v>249</v>
+        <v>58.45554302122859</v>
       </c>
       <c r="AZ8" t="n">
-        <v>307</v>
+        <v>59.8369957701434</v>
       </c>
       <c r="BA8" t="n">
-        <v>386</v>
+        <v>82.17183274391512</v>
       </c>
       <c r="BB8" t="n">
-        <v>466</v>
+        <v>83.91021606880638</v>
       </c>
       <c r="BC8" t="n">
-        <v>559</v>
+        <v>98.50651414045123</v>
       </c>
       <c r="BD8" t="n">
-        <v>670</v>
+        <v>118.9710610932476</v>
       </c>
       <c r="BE8" t="n">
-        <v>821</v>
+        <v>164.5059374659549</v>
       </c>
       <c r="BF8" t="n">
-        <v>962</v>
+        <v>156.0079663642399</v>
       </c>
       <c r="BG8" t="n">
-        <v>1157</v>
+        <v>220.5134004297184</v>
       </c>
       <c r="BH8" t="n">
-        <v>1363</v>
+        <v>238.5087414611555</v>
       </c>
       <c r="BI8" t="n">
-        <v>1541</v>
+        <v>210.4267643929543</v>
       </c>
       <c r="BJ8" t="n">
-        <v>1759</v>
+        <v>264.5310035189904</v>
       </c>
       <c r="BK8" t="n">
-        <v>1987</v>
+        <v>284.5376263571696</v>
       </c>
       <c r="BL8" t="n">
-        <v>2259</v>
+        <v>351.3757912414417</v>
       </c>
       <c r="BM8" t="n">
-        <v>2559</v>
+        <v>403.1716167181831</v>
       </c>
       <c r="BN8" t="n">
-        <v>2864</v>
+        <v>427.4103139013453</v>
       </c>
       <c r="BO8" t="n">
-        <v>3214</v>
+        <v>515.7677571470675</v>
       </c>
       <c r="BP8" t="n">
-        <v>3573</v>
+        <v>558.5809864633577</v>
       </c>
       <c r="BQ8" t="n">
-        <v>3916</v>
+        <v>563.7738330046022</v>
       </c>
       <c r="BR8" t="n">
-        <v>4269</v>
+        <v>615.9483510731111</v>
       </c>
       <c r="BS8" t="n">
-        <v>4636</v>
+        <v>684.1909023117076</v>
       </c>
       <c r="BT8" t="n">
-        <v>5022</v>
+        <v>775.4118119726799</v>
       </c>
       <c r="BU8" t="n">
-        <v>5403</v>
+        <v>828.8013922123123</v>
       </c>
       <c r="BV8" t="n">
-        <v>5799</v>
+        <v>942.6327064984528</v>
       </c>
       <c r="BW8" t="n">
-        <v>6178</v>
+        <v>991.6274201988489</v>
       </c>
       <c r="BX8" t="n">
-        <v>6559</v>
+        <v>1107.236268526591</v>
       </c>
       <c r="BY8" t="n">
-        <v>6932</v>
+        <v>1215.775749674055</v>
       </c>
       <c r="BZ8" t="n">
-        <v>7304</v>
+        <v>1379.821958456973</v>
       </c>
       <c r="CA8" t="n">
-        <v>7684</v>
+        <v>1640.759930915371</v>
       </c>
       <c r="CB8" t="n">
-        <v>7966</v>
+        <v>1386.430678466077</v>
       </c>
       <c r="CC8" t="n">
-        <v>8292</v>
+        <v>1908.665105386417</v>
       </c>
       <c r="CD8" t="n">
-        <v>8562</v>
+        <v>1877.607788595271</v>
       </c>
       <c r="CE8" t="n">
-        <v>8804</v>
+        <v>2023.411371237458</v>
       </c>
       <c r="CF8" t="n">
-        <v>9019</v>
+        <v>2191.64118246687</v>
       </c>
       <c r="CG8" t="n">
-        <v>9201</v>
+        <v>2277.84730913642</v>
       </c>
       <c r="CH8" t="n">
-        <v>9378</v>
+        <v>2845.659163987138</v>
       </c>
       <c r="CI8" t="n">
-        <v>9506</v>
+        <v>2591.093117408907</v>
       </c>
       <c r="CJ8" t="n">
-        <v>9611</v>
+        <v>2699.228791773779</v>
       </c>
       <c r="CK8" t="n">
-        <v>9708</v>
+        <v>3321.917808219178</v>
       </c>
       <c r="CL8" t="n">
-        <v>9781</v>
+        <v>3333.333333333333</v>
       </c>
       <c r="CM8" t="n">
-        <v>9827</v>
+        <v>2658.959537572254</v>
       </c>
       <c r="CN8" t="n">
-        <v>9880</v>
+        <v>4416.666666666667</v>
       </c>
       <c r="CO8" t="n">
-        <v>9908</v>
+        <v>3043.478260869565</v>
       </c>
       <c r="CP8" t="n">
-        <v>9930</v>
+        <v>3142.857142857143</v>
       </c>
       <c r="CQ8" t="n">
-        <v>9948</v>
+        <v>3461.538461538461</v>
       </c>
       <c r="CR8" t="n">
-        <v>9965</v>
+        <v>4857.142857142857</v>
       </c>
       <c r="CS8" t="n">
-        <v>9977</v>
+        <v>5217.391304347826</v>
       </c>
       <c r="CT8" t="n">
-        <v>9985</v>
+        <v>5333.333333333333</v>
       </c>
       <c r="CU8" t="n">
-        <v>9990</v>
+        <v>5000</v>
       </c>
       <c r="CV8" t="n">
-        <v>9993</v>
+        <v>4285.714285714285</v>
       </c>
       <c r="CW8" t="n">
-        <v>9995</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="9" spans="1:101">
@@ -2909,215 +2912,199 @@
         <v>0</v>
       </c>
       <c r="AF9" t="n">
-        <v>3</v>
+        <v>3.000900270081024</v>
       </c>
       <c r="AG9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AH9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AI9" t="n">
-        <v>5</v>
+        <v>2.001000500250125</v>
       </c>
       <c r="AJ9" t="n">
-        <v>9</v>
+        <v>4.003603242918627</v>
       </c>
       <c r="AK9" t="n">
-        <v>14</v>
+        <v>5.007009813739235</v>
       </c>
       <c r="AL9" t="n">
-        <v>22</v>
+        <v>8.017638805371819</v>
       </c>
       <c r="AM9" t="n">
-        <v>27</v>
+        <v>5.01353654868144</v>
       </c>
       <c r="AN9" t="n">
-        <v>33</v>
+        <v>6.019865556335909</v>
       </c>
       <c r="AO9" t="n">
-        <v>47</v>
+        <v>14.06611072038581</v>
       </c>
       <c r="AP9" t="n">
-        <v>52</v>
+        <v>5.026135906714917</v>
       </c>
       <c r="AQ9" t="n">
-        <v>69</v>
+        <v>17.11811499345484</v>
       </c>
       <c r="AR9" t="n">
-        <v>95</v>
+        <v>26.24936900555275</v>
       </c>
       <c r="AS9" t="n">
-        <v>128</v>
+        <v>33.42787682333874</v>
       </c>
       <c r="AT9" t="n">
-        <v>177</v>
+        <v>49.8829278224575</v>
       </c>
       <c r="AU9" t="n">
-        <v>232</v>
+        <v>56.3063063063063</v>
       </c>
       <c r="AV9" t="n">
-        <v>298</v>
+        <v>68.02721088435374</v>
       </c>
       <c r="AW9" t="n">
-        <v>392</v>
+        <v>97.83513738551207</v>
       </c>
       <c r="AX9" t="n">
-        <v>501</v>
+        <v>114.7489209390462</v>
       </c>
       <c r="AY9" t="n">
-        <v>633</v>
+        <v>140.9202519483292</v>
       </c>
       <c r="AZ9" t="n">
-        <v>790</v>
+        <v>170.4668838219327</v>
       </c>
       <c r="BA9" t="n">
-        <v>941</v>
+        <v>166.6850645766641</v>
       </c>
       <c r="BB9" t="n">
-        <v>1160</v>
+        <v>247.737556561086</v>
       </c>
       <c r="BC9" t="n">
-        <v>1399</v>
+        <v>277.8746657365422</v>
       </c>
       <c r="BD9" t="n">
-        <v>1663</v>
+        <v>316.6606693055056</v>
       </c>
       <c r="BE9" t="n">
-        <v>1974</v>
+        <v>387.4906553700473</v>
       </c>
       <c r="BF9" t="n">
-        <v>2318</v>
+        <v>447.8000520697735</v>
       </c>
       <c r="BG9" t="n">
-        <v>2651</v>
+        <v>453.1228738603892</v>
       </c>
       <c r="BH9" t="n">
-        <v>2996</v>
+        <v>492.5756710451171</v>
       </c>
       <c r="BI9" t="n">
-        <v>3339</v>
+        <v>514.9376970424861</v>
       </c>
       <c r="BJ9" t="n">
-        <v>3737</v>
+        <v>635.4782053329075</v>
       </c>
       <c r="BK9" t="n">
-        <v>4150</v>
+        <v>705.9829059829059</v>
       </c>
       <c r="BL9" t="n">
-        <v>4582</v>
+        <v>797.3421926910298</v>
       </c>
       <c r="BM9" t="n">
-        <v>5015</v>
+        <v>868.6058174523571</v>
       </c>
       <c r="BN9" t="n">
-        <v>5464</v>
+        <v>989.8589065255732</v>
       </c>
       <c r="BO9" t="n">
-        <v>5889</v>
+        <v>1033.811724641206</v>
       </c>
       <c r="BP9" t="n">
-        <v>6327</v>
+        <v>1192.485706506943</v>
       </c>
       <c r="BQ9" t="n">
-        <v>6724</v>
+        <v>1211.843711843712</v>
       </c>
       <c r="BR9" t="n">
-        <v>7097</v>
+        <v>1284.877712710989</v>
       </c>
       <c r="BS9" t="n">
-        <v>7455</v>
+        <v>1406.679764243615</v>
       </c>
       <c r="BT9" t="n">
-        <v>7818</v>
+        <v>1663.611365719523</v>
       </c>
       <c r="BU9" t="n">
-        <v>8144</v>
+        <v>1756.465517241379</v>
       </c>
       <c r="BV9" t="n">
-        <v>8464</v>
+        <v>2083.333333333333</v>
       </c>
       <c r="BW9" t="n">
-        <v>8714</v>
+        <v>1944.012441679627</v>
       </c>
       <c r="BX9" t="n">
-        <v>8955</v>
+        <v>2306.22009569378</v>
       </c>
       <c r="BY9" t="n">
-        <v>9153</v>
+        <v>2337.662337662337</v>
       </c>
       <c r="BZ9" t="n">
-        <v>9320</v>
+        <v>2455.882352941176</v>
       </c>
       <c r="CA9" t="n">
-        <v>9455</v>
+        <v>2477.064220183486</v>
       </c>
       <c r="CB9" t="n">
-        <v>9597</v>
+        <v>3523.573200992556</v>
       </c>
       <c r="CC9" t="n">
-        <v>9681</v>
+        <v>2633.228840125392</v>
       </c>
       <c r="CD9" t="n">
-        <v>9774</v>
+        <v>4115.04424778761</v>
       </c>
       <c r="CE9" t="n">
-        <v>9836</v>
+        <v>3780.487804878049</v>
       </c>
       <c r="CF9" t="n">
-        <v>9881</v>
+        <v>3781.512605042017</v>
       </c>
       <c r="CG9" t="n">
-        <v>9909</v>
+        <v>3076.923076923077</v>
       </c>
       <c r="CH9" t="n">
-        <v>9940</v>
+        <v>5166.666666666667</v>
       </c>
       <c r="CI9" t="n">
-        <v>9962</v>
+        <v>5789.473684210527</v>
       </c>
       <c r="CJ9" t="n">
-        <v>9977</v>
+        <v>6521.739130434783</v>
       </c>
       <c r="CK9" t="n">
-        <v>9986</v>
+        <v>6428.571428571429</v>
       </c>
       <c r="CL9" t="n">
-        <v>9995</v>
+        <v>18000</v>
       </c>
       <c r="CM9" t="n">
-        <v>9996</v>
+        <v>2500</v>
       </c>
       <c r="CN9" t="n">
-        <v>9997</v>
-      </c>
-      <c r="CO9" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CP9" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CQ9" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CR9" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CS9" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CT9" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CU9" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CV9" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CW9" t="n">
-        <v>10000</v>
-      </c>
+        <v>3333.333333333333</v>
+      </c>
+      <c r="CO9" t="s">
+        <v>1</v>
+      </c>
+      <c r="CP9" t="s"/>
+      <c r="CQ9" t="s"/>
+      <c r="CR9" t="s"/>
+      <c r="CS9" t="s"/>
+      <c r="CT9" t="s"/>
+      <c r="CU9" t="s"/>
+      <c r="CV9" t="s"/>
+      <c r="CW9" t="s"/>
     </row>
     <row r="10" spans="1:101">
       <c r="A10" s="1" t="n">
@@ -3202,227 +3189,193 @@
         <v>0</v>
       </c>
       <c r="AB10" t="n">
+        <v>1.000100010001</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>1.000200040008002</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>1.000300090027008</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>1.000400160064026</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>3.002101471029721</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>1.00080064051241</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>2.002002002002002</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>6.009615384615385</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>10.02606777621817</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>8.027292795504716</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>17.0871444366268</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>23.1714688696353</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>20.18978396931153</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>36.4741641337386</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>44.77915733767555</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>65.56033599672199</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>85.75266039880152</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>102.285773927565</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>126.8364866293204</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>175.3065175306517</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>224.3237299318232</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>238.6849808601666</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>318.3085501858736</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>348.6415003606636</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>402.7013506753377</v>
+      </c>
+      <c r="BA10" t="n">
+        <v>541.8589321028346</v>
+      </c>
+      <c r="BB10" t="n">
+        <v>530.3345828127169</v>
+      </c>
+      <c r="BC10" t="n">
+        <v>685.3582554517134</v>
+      </c>
+      <c r="BD10" t="n">
+        <v>758.0593680178741</v>
+      </c>
+      <c r="BE10" t="n">
+        <v>784.8537005163511</v>
+      </c>
+      <c r="BF10" t="n">
+        <v>1010.043585370476</v>
+      </c>
+      <c r="BG10" t="n">
+        <v>968.613593847433</v>
+      </c>
+      <c r="BH10" t="n">
+        <v>1214.452214452215</v>
+      </c>
+      <c r="BI10" t="n">
+        <v>1337.209302325581</v>
+      </c>
+      <c r="BJ10" t="n">
+        <v>1278.688524590164</v>
+      </c>
+      <c r="BK10" t="n">
+        <v>1537.138927097662</v>
+      </c>
+      <c r="BL10" t="n">
+        <v>1869.387755102041</v>
+      </c>
+      <c r="BM10" t="n">
+        <v>1700.095510983763</v>
+      </c>
+      <c r="BN10" t="n">
+        <v>2000</v>
+      </c>
+      <c r="BO10" t="n">
+        <v>2118.055555555556</v>
+      </c>
+      <c r="BP10" t="n">
+        <v>2413.793103448276</v>
+      </c>
+      <c r="BQ10" t="n">
+        <v>2108.559498956159</v>
+      </c>
+      <c r="BR10" t="n">
+        <v>2588.699080157687</v>
+      </c>
+      <c r="BS10" t="n">
+        <v>3188.908145580589</v>
+      </c>
+      <c r="BT10" t="n">
+        <v>3387.470997679814</v>
+      </c>
+      <c r="BU10" t="n">
+        <v>3903.225806451613</v>
+      </c>
+      <c r="BV10" t="n">
+        <v>3478.260869565217</v>
+      </c>
+      <c r="BW10" t="n">
+        <v>3609.467455621302</v>
+      </c>
+      <c r="BX10" t="n">
+        <v>5363.636363636364</v>
+      </c>
+      <c r="BY10" t="n">
+        <v>5068.493150684932</v>
+      </c>
+      <c r="BZ10" t="n">
+        <v>4038.461538461539</v>
+      </c>
+      <c r="CA10" t="n">
+        <v>6250</v>
+      </c>
+      <c r="CB10" t="n">
+        <v>6842.105263157895</v>
+      </c>
+      <c r="CC10" t="n">
+        <v>7272.727272727273</v>
+      </c>
+      <c r="CD10" t="n">
+        <v>5714.285714285714</v>
+      </c>
+      <c r="CE10" t="n">
+        <v>25000</v>
+      </c>
+      <c r="CF10" t="s">
         <v>1</v>
       </c>
-      <c r="AC10" t="n">
-        <v>2</v>
-      </c>
-      <c r="AD10" t="n">
-        <v>3</v>
-      </c>
-      <c r="AE10" t="n">
-        <v>4</v>
-      </c>
-      <c r="AF10" t="n">
-        <v>7</v>
-      </c>
-      <c r="AG10" t="n">
-        <v>8</v>
-      </c>
-      <c r="AH10" t="n">
-        <v>10</v>
-      </c>
-      <c r="AI10" t="n">
-        <v>16</v>
-      </c>
-      <c r="AJ10" t="n">
-        <v>26</v>
-      </c>
-      <c r="AK10" t="n">
-        <v>34</v>
-      </c>
-      <c r="AL10" t="n">
-        <v>51</v>
-      </c>
-      <c r="AM10" t="n">
-        <v>74</v>
-      </c>
-      <c r="AN10" t="n">
-        <v>94</v>
-      </c>
-      <c r="AO10" t="n">
-        <v>130</v>
-      </c>
-      <c r="AP10" t="n">
-        <v>174</v>
-      </c>
-      <c r="AQ10" t="n">
-        <v>238</v>
-      </c>
-      <c r="AR10" t="n">
-        <v>321</v>
-      </c>
-      <c r="AS10" t="n">
-        <v>419</v>
-      </c>
-      <c r="AT10" t="n">
-        <v>539</v>
-      </c>
-      <c r="AU10" t="n">
-        <v>702</v>
-      </c>
-      <c r="AV10" t="n">
-        <v>906</v>
-      </c>
-      <c r="AW10" t="n">
-        <v>1118</v>
-      </c>
-      <c r="AX10" t="n">
-        <v>1392</v>
-      </c>
-      <c r="AY10" t="n">
-        <v>1682</v>
-      </c>
-      <c r="AZ10" t="n">
-        <v>2004</v>
-      </c>
-      <c r="BA10" t="n">
-        <v>2415</v>
-      </c>
-      <c r="BB10" t="n">
-        <v>2797</v>
-      </c>
-      <c r="BC10" t="n">
-        <v>3259</v>
-      </c>
-      <c r="BD10" t="n">
-        <v>3734</v>
-      </c>
-      <c r="BE10" t="n">
-        <v>4190</v>
-      </c>
-      <c r="BF10" t="n">
-        <v>4723</v>
-      </c>
-      <c r="BG10" t="n">
-        <v>5189</v>
-      </c>
-      <c r="BH10" t="n">
-        <v>5710</v>
-      </c>
-      <c r="BI10" t="n">
-        <v>6216</v>
-      </c>
-      <c r="BJ10" t="n">
-        <v>6645</v>
-      </c>
-      <c r="BK10" t="n">
-        <v>7092</v>
-      </c>
-      <c r="BL10" t="n">
-        <v>7550</v>
-      </c>
-      <c r="BM10" t="n">
-        <v>7906</v>
-      </c>
-      <c r="BN10" t="n">
-        <v>8255</v>
-      </c>
-      <c r="BO10" t="n">
-        <v>8560</v>
-      </c>
-      <c r="BP10" t="n">
-        <v>8840</v>
-      </c>
-      <c r="BQ10" t="n">
-        <v>9042</v>
-      </c>
-      <c r="BR10" t="n">
-        <v>9239</v>
-      </c>
-      <c r="BS10" t="n">
-        <v>9423</v>
-      </c>
-      <c r="BT10" t="n">
-        <v>9569</v>
-      </c>
-      <c r="BU10" t="n">
-        <v>9690</v>
-      </c>
-      <c r="BV10" t="n">
-        <v>9770</v>
-      </c>
-      <c r="BW10" t="n">
-        <v>9831</v>
-      </c>
-      <c r="BX10" t="n">
-        <v>9890</v>
-      </c>
-      <c r="BY10" t="n">
-        <v>9927</v>
-      </c>
-      <c r="BZ10" t="n">
-        <v>9948</v>
-      </c>
-      <c r="CA10" t="n">
-        <v>9968</v>
-      </c>
-      <c r="CB10" t="n">
-        <v>9981</v>
-      </c>
-      <c r="CC10" t="n">
-        <v>9989</v>
-      </c>
-      <c r="CD10" t="n">
-        <v>9993</v>
-      </c>
-      <c r="CE10" t="n">
-        <v>9998</v>
-      </c>
-      <c r="CF10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CG10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CH10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CI10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CJ10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CK10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CL10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CM10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CN10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CO10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CP10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CQ10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CR10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CS10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CT10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CU10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CV10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CW10" t="n">
-        <v>10000</v>
-      </c>
+      <c r="CG10" t="s"/>
+      <c r="CH10" t="s"/>
+      <c r="CI10" t="s"/>
+      <c r="CJ10" t="s"/>
+      <c r="CK10" t="s"/>
+      <c r="CL10" t="s"/>
+      <c r="CM10" t="s"/>
+      <c r="CN10" t="s"/>
+      <c r="CO10" t="s"/>
+      <c r="CP10" t="s"/>
+      <c r="CQ10" t="s"/>
+      <c r="CR10" t="s"/>
+      <c r="CS10" t="s"/>
+      <c r="CT10" t="s"/>
+      <c r="CU10" t="s"/>
+      <c r="CV10" t="s"/>
+      <c r="CW10" t="s"/>
     </row>
     <row r="11" spans="1:101">
       <c r="A11" s="1" t="n">
@@ -3492,242 +3445,206 @@
         <v>0</v>
       </c>
       <c r="W11" t="n">
+        <v>1.000100010001</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>2.000600180054016</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>1.000400160064026</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>1.000500250125063</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>2.001400980686481</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>4.004404845329863</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>3.004205888243541</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>1.00150225338007</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>11.02867455383998</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>8.027292795504716</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>10.04419445560466</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>23.1551394342092</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>45.50970873786407</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>37.559638615369</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>44.86591210359947</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>60.52523594583504</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>81.70441617540594</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>105.5602006688963</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>147.4175416268957</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>184.7051198963059</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>236.6209641751437</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>272.6033621081327</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>388.2005899705015</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>403.8792045175546</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>528.628667442161</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>576.8967874231032</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>746.2905832231527</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>912.1513305546649</v>
+      </c>
+      <c r="BA11" t="n">
+        <v>974.6657283603097</v>
+      </c>
+      <c r="BB11" t="n">
+        <v>1213.257052673111</v>
+      </c>
+      <c r="BC11" t="n">
+        <v>1324.843610366398</v>
+      </c>
+      <c r="BD11" t="n">
+        <v>1577.858251422659</v>
+      </c>
+      <c r="BE11" t="n">
+        <v>1648.086773124435</v>
+      </c>
+      <c r="BF11" t="n">
+        <v>1934.55591513844</v>
+      </c>
+      <c r="BG11" t="n">
+        <v>2234.931808183018</v>
+      </c>
+      <c r="BH11" t="n">
+        <v>2564.953012714207</v>
+      </c>
+      <c r="BI11" t="n">
+        <v>2685.834502103787</v>
+      </c>
+      <c r="BJ11" t="n">
+        <v>2999.088422971741</v>
+      </c>
+      <c r="BK11" t="n">
+        <v>3200.962695547533</v>
+      </c>
+      <c r="BL11" t="n">
+        <v>3600.654664484452</v>
+      </c>
+      <c r="BM11" t="n">
+        <v>3699.551569506727</v>
+      </c>
+      <c r="BN11" t="n">
+        <v>3808.049535603715</v>
+      </c>
+      <c r="BO11" t="n">
+        <v>5756.09756097561</v>
+      </c>
+      <c r="BP11" t="n">
+        <v>3225.806451612903</v>
+      </c>
+      <c r="BQ11" t="n">
+        <v>5656.565656565656</v>
+      </c>
+      <c r="BR11" t="n">
+        <v>5714.285714285714</v>
+      </c>
+      <c r="BS11" t="n">
+        <v>7500</v>
+      </c>
+      <c r="BT11" t="n">
+        <v>3333.333333333333</v>
+      </c>
+      <c r="BU11" t="n">
+        <v>8000</v>
+      </c>
+      <c r="BV11" t="n">
+        <v>6666.666666666666</v>
+      </c>
+      <c r="BW11" t="n">
+        <v>5000</v>
+      </c>
+      <c r="BX11" t="n">
+        <v>5000</v>
+      </c>
+      <c r="BY11" t="n">
+        <v>0</v>
+      </c>
+      <c r="BZ11" t="n">
+        <v>3333.333333333333</v>
+      </c>
+      <c r="CA11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CB11" t="n">
+        <v>20000</v>
+      </c>
+      <c r="CC11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD11" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE11" t="s">
         <v>1</v>
       </c>
-      <c r="X11" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>4</v>
-      </c>
-      <c r="AB11" t="n">
-        <v>5</v>
-      </c>
-      <c r="AC11" t="n">
-        <v>7</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>11</v>
-      </c>
-      <c r="AE11" t="n">
-        <v>14</v>
-      </c>
-      <c r="AF11" t="n">
-        <v>15</v>
-      </c>
-      <c r="AG11" t="n">
-        <v>26</v>
-      </c>
-      <c r="AH11" t="n">
-        <v>34</v>
-      </c>
-      <c r="AI11" t="n">
-        <v>44</v>
-      </c>
-      <c r="AJ11" t="n">
-        <v>67</v>
-      </c>
-      <c r="AK11" t="n">
-        <v>112</v>
-      </c>
-      <c r="AL11" t="n">
-        <v>149</v>
-      </c>
-      <c r="AM11" t="n">
-        <v>193</v>
-      </c>
-      <c r="AN11" t="n">
-        <v>252</v>
-      </c>
-      <c r="AO11" t="n">
-        <v>331</v>
-      </c>
-      <c r="AP11" t="n">
-        <v>432</v>
-      </c>
-      <c r="AQ11" t="n">
-        <v>571</v>
-      </c>
-      <c r="AR11" t="n">
-        <v>742</v>
-      </c>
-      <c r="AS11" t="n">
-        <v>956</v>
-      </c>
-      <c r="AT11" t="n">
-        <v>1196</v>
-      </c>
-      <c r="AU11" t="n">
-        <v>1525</v>
-      </c>
-      <c r="AV11" t="n">
-        <v>1854</v>
-      </c>
-      <c r="AW11" t="n">
-        <v>2263</v>
-      </c>
-      <c r="AX11" t="n">
-        <v>2685</v>
-      </c>
-      <c r="AY11" t="n">
-        <v>3193</v>
-      </c>
-      <c r="AZ11" t="n">
-        <v>3762</v>
-      </c>
-      <c r="BA11" t="n">
-        <v>4316</v>
-      </c>
-      <c r="BB11" t="n">
-        <v>4931</v>
-      </c>
-      <c r="BC11" t="n">
-        <v>5524</v>
-      </c>
-      <c r="BD11" t="n">
-        <v>6134</v>
-      </c>
-      <c r="BE11" t="n">
-        <v>6681</v>
-      </c>
-      <c r="BF11" t="n">
-        <v>7219</v>
-      </c>
-      <c r="BG11" t="n">
-        <v>7727</v>
-      </c>
-      <c r="BH11" t="n">
-        <v>8191</v>
-      </c>
-      <c r="BI11" t="n">
-        <v>8574</v>
-      </c>
-      <c r="BJ11" t="n">
-        <v>8903</v>
-      </c>
-      <c r="BK11" t="n">
-        <v>9169</v>
-      </c>
-      <c r="BL11" t="n">
-        <v>9389</v>
-      </c>
-      <c r="BM11" t="n">
-        <v>9554</v>
-      </c>
-      <c r="BN11" t="n">
-        <v>9677</v>
-      </c>
-      <c r="BO11" t="n">
-        <v>9795</v>
-      </c>
-      <c r="BP11" t="n">
-        <v>9845</v>
-      </c>
-      <c r="BQ11" t="n">
-        <v>9901</v>
-      </c>
-      <c r="BR11" t="n">
-        <v>9937</v>
-      </c>
-      <c r="BS11" t="n">
-        <v>9964</v>
-      </c>
-      <c r="BT11" t="n">
-        <v>9973</v>
-      </c>
-      <c r="BU11" t="n">
-        <v>9985</v>
-      </c>
-      <c r="BV11" t="n">
-        <v>9991</v>
-      </c>
-      <c r="BW11" t="n">
-        <v>9994</v>
-      </c>
-      <c r="BX11" t="n">
-        <v>9996</v>
-      </c>
-      <c r="BY11" t="n">
-        <v>9996</v>
-      </c>
-      <c r="BZ11" t="n">
-        <v>9997</v>
-      </c>
-      <c r="CA11" t="n">
-        <v>9997</v>
-      </c>
-      <c r="CB11" t="n">
-        <v>9999</v>
-      </c>
-      <c r="CC11" t="n">
-        <v>9999</v>
-      </c>
-      <c r="CD11" t="n">
-        <v>9999</v>
-      </c>
-      <c r="CE11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CF11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CG11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CH11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CI11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CJ11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CK11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CL11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CM11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CN11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CO11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CP11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CQ11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CR11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CS11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CT11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CU11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CV11" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CW11" t="n">
-        <v>10000</v>
-      </c>
+      <c r="CF11" t="s"/>
+      <c r="CG11" t="s"/>
+      <c r="CH11" t="s"/>
+      <c r="CI11" t="s"/>
+      <c r="CJ11" t="s"/>
+      <c r="CK11" t="s"/>
+      <c r="CL11" t="s"/>
+      <c r="CM11" t="s"/>
+      <c r="CN11" t="s"/>
+      <c r="CO11" t="s"/>
+      <c r="CP11" t="s"/>
+      <c r="CQ11" t="s"/>
+      <c r="CR11" t="s"/>
+      <c r="CS11" t="s"/>
+      <c r="CT11" t="s"/>
+      <c r="CU11" t="s"/>
+      <c r="CV11" t="s"/>
+      <c r="CW11" t="s"/>
     </row>
     <row r="12" spans="1:101">
       <c r="A12" s="1" t="n">
@@ -3782,257 +3699,203 @@
         <v>0</v>
       </c>
       <c r="R12" t="n">
+        <v>1.000100010001</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>2.000600180054016</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>2.001000500250125</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>4.003603242918627</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>7.011217948717949</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>8.019246190858059</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>17.06998694648057</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>10.05126143330988</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>23.1714688696353</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>33.35691903366016</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>36.52226843867302</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>59.18971323604449</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>59.54214146391541</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>78.63424728401449</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>113.0061734854034</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>144.3583483706613</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>173.866090712743</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>228.6534850325859</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>279.3232655841944</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>373.3804475853946</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>447.9448683238986</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>561.4764751754614</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>650.609080841639</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>887.7166541070084</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>1034.425411608182</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>1147.571375602521</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>1435.234259062964</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>1652.667984189723</v>
+      </c>
+      <c r="BA12" t="n">
+        <v>1990.521327014218</v>
+      </c>
+      <c r="BB12" t="n">
+        <v>2334.672999634637</v>
+      </c>
+      <c r="BC12" t="n">
+        <v>2589.696412143514</v>
+      </c>
+      <c r="BD12" t="n">
+        <v>2940.47619047619</v>
+      </c>
+      <c r="BE12" t="n">
+        <v>3003.095975232198</v>
+      </c>
+      <c r="BF12" t="n">
+        <v>3671.957671957672</v>
+      </c>
+      <c r="BG12" t="n">
+        <v>4427.480916030535</v>
+      </c>
+      <c r="BH12" t="n">
+        <v>5375.586854460093</v>
+      </c>
+      <c r="BI12" t="n">
+        <v>4589.041095890411</v>
+      </c>
+      <c r="BJ12" t="n">
+        <v>4822.33502538071</v>
+      </c>
+      <c r="BK12" t="n">
+        <v>7747.747747747748</v>
+      </c>
+      <c r="BL12" t="n">
+        <v>9473.684210526315</v>
+      </c>
+      <c r="BM12" t="n">
+        <v>6764.705882352941</v>
+      </c>
+      <c r="BN12" t="n">
+        <v>11250</v>
+      </c>
+      <c r="BO12" t="n">
+        <v>12857.14285714286</v>
+      </c>
+      <c r="BP12" t="n">
+        <v>1666.666666666667</v>
+      </c>
+      <c r="BQ12" t="n">
+        <v>10000</v>
+      </c>
+      <c r="BR12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="BS12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BU12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BV12" t="s">
         <v>1</v>
       </c>
-      <c r="S12" t="n">
-        <v>1</v>
-      </c>
-      <c r="T12" t="n">
-        <v>1</v>
-      </c>
-      <c r="U12" t="n">
-        <v>1</v>
-      </c>
-      <c r="V12" t="n">
-        <v>1</v>
-      </c>
-      <c r="W12" t="n">
-        <v>1</v>
-      </c>
-      <c r="X12" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB12" t="n">
-        <v>9</v>
-      </c>
-      <c r="AC12" t="n">
-        <v>16</v>
-      </c>
-      <c r="AD12" t="n">
-        <v>24</v>
-      </c>
-      <c r="AE12" t="n">
-        <v>41</v>
-      </c>
-      <c r="AF12" t="n">
-        <v>51</v>
-      </c>
-      <c r="AG12" t="n">
-        <v>74</v>
-      </c>
-      <c r="AH12" t="n">
-        <v>107</v>
-      </c>
-      <c r="AI12" t="n">
-        <v>143</v>
-      </c>
-      <c r="AJ12" t="n">
-        <v>201</v>
-      </c>
-      <c r="AK12" t="n">
-        <v>259</v>
-      </c>
-      <c r="AL12" t="n">
-        <v>335</v>
-      </c>
-      <c r="AM12" t="n">
-        <v>443</v>
-      </c>
-      <c r="AN12" t="n">
-        <v>579</v>
-      </c>
-      <c r="AO12" t="n">
-        <v>740</v>
-      </c>
-      <c r="AP12" t="n">
-        <v>947</v>
-      </c>
-      <c r="AQ12" t="n">
-        <v>1193</v>
-      </c>
-      <c r="AR12" t="n">
-        <v>1510</v>
-      </c>
-      <c r="AS12" t="n">
-        <v>1874</v>
-      </c>
-      <c r="AT12" t="n">
-        <v>2306</v>
-      </c>
-      <c r="AU12" t="n">
-        <v>2776</v>
-      </c>
-      <c r="AV12" t="n">
-        <v>3365</v>
-      </c>
-      <c r="AW12" t="n">
-        <v>3987</v>
-      </c>
-      <c r="AX12" t="n">
-        <v>4606</v>
-      </c>
-      <c r="AY12" t="n">
-        <v>5283</v>
-      </c>
-      <c r="AZ12" t="n">
-        <v>5952</v>
-      </c>
-      <c r="BA12" t="n">
-        <v>6624</v>
-      </c>
-      <c r="BB12" t="n">
-        <v>7263</v>
-      </c>
-      <c r="BC12" t="n">
-        <v>7826</v>
-      </c>
-      <c r="BD12" t="n">
-        <v>8320</v>
-      </c>
-      <c r="BE12" t="n">
-        <v>8708</v>
-      </c>
-      <c r="BF12" t="n">
-        <v>9055</v>
-      </c>
-      <c r="BG12" t="n">
-        <v>9345</v>
-      </c>
-      <c r="BH12" t="n">
-        <v>9574</v>
-      </c>
-      <c r="BI12" t="n">
-        <v>9708</v>
-      </c>
-      <c r="BJ12" t="n">
-        <v>9803</v>
-      </c>
-      <c r="BK12" t="n">
-        <v>9889</v>
-      </c>
-      <c r="BL12" t="n">
-        <v>9943</v>
-      </c>
-      <c r="BM12" t="n">
-        <v>9966</v>
-      </c>
-      <c r="BN12" t="n">
-        <v>9984</v>
-      </c>
-      <c r="BO12" t="n">
-        <v>9993</v>
-      </c>
-      <c r="BP12" t="n">
-        <v>9994</v>
-      </c>
-      <c r="BQ12" t="n">
-        <v>9997</v>
-      </c>
-      <c r="BR12" t="n">
-        <v>9999</v>
-      </c>
-      <c r="BS12" t="n">
-        <v>9999</v>
-      </c>
-      <c r="BT12" t="n">
-        <v>9999</v>
-      </c>
-      <c r="BU12" t="n">
-        <v>9999</v>
-      </c>
-      <c r="BV12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="BW12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="BX12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="BY12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="BZ12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CA12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CB12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CC12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CD12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CE12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CF12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CG12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CH12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CI12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CJ12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CK12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CL12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CM12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CN12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CO12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CP12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CQ12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CR12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CS12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CT12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CU12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CV12" t="n">
-        <v>10000</v>
-      </c>
-      <c r="CW12" t="n">
-        <v>10000</v>
-      </c>
+      <c r="BW12" t="s"/>
+      <c r="BX12" t="s"/>
+      <c r="BY12" t="s"/>
+      <c r="BZ12" t="s"/>
+      <c r="CA12" t="s"/>
+      <c r="CB12" t="s"/>
+      <c r="CC12" t="s"/>
+      <c r="CD12" t="s"/>
+      <c r="CE12" t="s"/>
+      <c r="CF12" t="s"/>
+      <c r="CG12" t="s"/>
+      <c r="CH12" t="s"/>
+      <c r="CI12" t="s"/>
+      <c r="CJ12" t="s"/>
+      <c r="CK12" t="s"/>
+      <c r="CL12" t="s"/>
+      <c r="CM12" t="s"/>
+      <c r="CN12" t="s"/>
+      <c r="CO12" t="s"/>
+      <c r="CP12" t="s"/>
+      <c r="CQ12" t="s"/>
+      <c r="CR12" t="s"/>
+      <c r="CS12" t="s"/>
+      <c r="CT12" t="s"/>
+      <c r="CU12" t="s"/>
+      <c r="CV12" t="s"/>
+      <c r="CW12" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>